<commit_message>
more work on pandas
</commit_message>
<xml_diff>
--- a/IDKY/TeamWorx/MySchedule_Jan26_Feb01.xlsx
+++ b/IDKY/TeamWorx/MySchedule_Jan26_Feb01.xlsx
@@ -17,9 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Location</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t/>
   </si>
   <si>
     <t>01/17/2026 15:07</t>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Hrs</t>
-  </si>
-  <si>
-    <t>13104 - Lehi (UT)</t>
   </si>
   <si>
     <t>Wednesday 01/28</t>
@@ -100,7 +97,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -169,11 +166,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -188,6 +188,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -509,14 +512,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="3.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="35.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="3.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="3.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="3.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="35.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="3.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="3.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -524,138 +527,138 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1"/>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1"/>
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="H10" s="1"/>
     </row>

</xml_diff>